<commit_message>
xlsx file new format
</commit_message>
<xml_diff>
--- a/Backend/Data/CSEMockExamQuestionsData.xlsx
+++ b/Backend/Data/CSEMockExamQuestionsData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">questions</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paragraph</t>
   </si>
 </sst>
 </file>
@@ -239,10 +242,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -265,6 +268,9 @@
       </c>
       <c r="F1" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>